<commit_message>
some logistic regression drafts + fisher comparison
</commit_message>
<xml_diff>
--- a/2023_sats_providers.xlsx
+++ b/2023_sats_providers.xlsx
@@ -1,119 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m296398\Desktop\no_show_stats\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0E16C0-950E-4CE2-9871-7FFDEBC1F8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="20775" yWindow="765" windowWidth="17715" windowHeight="18930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
-  <si>
-    <t>UniqueValues.appt.schdlng.prvdr</t>
-  </si>
-  <si>
-    <t>UniqueValues.appt.schdlng.prvdr.spclty</t>
-  </si>
-  <si>
-    <t>MAMMO</t>
-  </si>
-  <si>
-    <t>Diagnostic Radiology</t>
-  </si>
-  <si>
-    <t>CREIGHTON_FM</t>
-  </si>
-  <si>
-    <t>Family Medicine</t>
-  </si>
-  <si>
-    <t>Sports_Physicals</t>
-  </si>
-  <si>
-    <t>JONES_DOUGLAS</t>
-  </si>
-  <si>
-    <t>Edward_Paul</t>
-  </si>
-  <si>
-    <t>STOUT_M</t>
-  </si>
-  <si>
-    <t>MORAN_A</t>
-  </si>
-  <si>
-    <t>Infectious Disease</t>
-  </si>
-  <si>
-    <t>CREIGHTON_IM</t>
-  </si>
-  <si>
-    <t>Internal Medicine</t>
-  </si>
-  <si>
-    <t>ECHO</t>
-  </si>
-  <si>
-    <t>Laboratory Medicine/Diagnostics</t>
-  </si>
-  <si>
-    <t>~LAB</t>
-  </si>
-  <si>
-    <t>~TB</t>
-  </si>
-  <si>
-    <t>RETINAL_SCAN</t>
-  </si>
-  <si>
-    <t>Ophthalmology/Optometry</t>
-  </si>
-  <si>
-    <t>CHURGIN_D</t>
-  </si>
-  <si>
-    <t>CREIGHTON_PEDS</t>
-  </si>
-  <si>
-    <t>Pediatric Medicine</t>
-  </si>
-  <si>
-    <t>SPENCER_W</t>
-  </si>
-  <si>
-    <t>Psychiatry/Psychology</t>
-  </si>
-  <si>
-    <t>GRADO_G</t>
-  </si>
-  <si>
-    <t>Radiation Oncology</t>
-  </si>
-  <si>
-    <t>KALLINGAL_G</t>
-  </si>
-  <si>
-    <t>Urology</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">UniqueValues.appt.schdlng.prvdr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniqueValues.appt.schdlng.prvdr.spclty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAMMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostic Radiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREIGHTON_FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family Medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports_Physicals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JONES_DOUGLAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edward_Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOUT_M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORAN_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infectious Disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREIGHTON_IM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratory Medicine/Diagnostics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~TB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETINAL_SCAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ophthalmology/Optometry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHURGIN_D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREIGHTON_PEDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pediatric Medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPENCER_W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psychiatry/Psychology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRADO_G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiation Oncology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KALLINGAL_G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -130,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -138,48 +131,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -461,36 +423,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -498,7 +454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -506,7 +462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -514,7 +470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -522,31 +478,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -554,7 +510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -562,15 +518,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -578,39 +534,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -620,12 +576,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{11372f5f-8e19-4efb-8afe-8eac20a980c4}" enabled="1" method="Standard" siteId="{a25fff9c-3f63-4fb2-9a8a-d9bdd0321f9a}" contentBits="0" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>